<commit_message>
third commit : 1st April 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6F509F-72B9-4A29-88F7-3842BF622E38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE95745-F323-4A8C-9C52-63347BF03C4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1865,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" zoomScale="78" workbookViewId="0">
-      <selection activeCell="B186" sqref="B186"/>
+    <sheetView tabSelected="1" topLeftCell="A191" zoomScale="78" workbookViewId="0">
+      <selection activeCell="B206" sqref="B206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -4541,7 +4541,7 @@
       <c r="A202">
         <v>187</v>
       </c>
-      <c r="B202" s="5" t="s">
+      <c r="B202" s="11" t="s">
         <v>171</v>
       </c>
       <c r="C202" s="6" t="s">
@@ -4597,7 +4597,7 @@
       <c r="A206">
         <v>191</v>
       </c>
-      <c r="B206" s="5" t="s">
+      <c r="B206" s="11" t="s">
         <v>171</v>
       </c>
       <c r="C206" s="6" t="s">
@@ -4611,7 +4611,7 @@
       <c r="A207">
         <v>192</v>
       </c>
-      <c r="B207" s="5" t="s">
+      <c r="B207" s="11" t="s">
         <v>171</v>
       </c>
       <c r="C207" s="6" t="s">

</xml_diff>

<commit_message>
4th commit : 12th April 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE95745-F323-4A8C-9C52-63347BF03C4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08523CC8-FC06-476A-B0E5-F726F90209C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1865,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" zoomScale="78" workbookViewId="0">
-      <selection activeCell="B206" sqref="B206"/>
+    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="78" workbookViewId="0">
+      <selection activeCell="B196" sqref="B196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -4457,7 +4457,7 @@
       <c r="A196">
         <v>181</v>
       </c>
-      <c r="B196" s="5" t="s">
+      <c r="B196" s="11" t="s">
         <v>171</v>
       </c>
       <c r="C196" s="6" t="s">
@@ -4583,7 +4583,7 @@
       <c r="A205">
         <v>190</v>
       </c>
-      <c r="B205" s="5" t="s">
+      <c r="B205" s="11" t="s">
         <v>171</v>
       </c>
       <c r="C205" s="6" t="s">
@@ -4639,7 +4639,7 @@
       <c r="A209">
         <v>194</v>
       </c>
-      <c r="B209" s="5" t="s">
+      <c r="B209" s="11" t="s">
         <v>171</v>
       </c>
       <c r="C209" s="6" t="s">

</xml_diff>

<commit_message>
5th commit : 30th April 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08523CC8-FC06-476A-B0E5-F726F90209C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3F91A3-87E6-46EE-AB80-076E8BC3BBC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1865,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="78" workbookViewId="0">
-      <selection activeCell="B196" sqref="B196"/>
+    <sheetView tabSelected="1" topLeftCell="A217" zoomScale="78" workbookViewId="0">
+      <selection activeCell="C234" sqref="C234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -4733,7 +4733,7 @@
       <c r="A217">
         <v>200</v>
       </c>
-      <c r="B217" s="5" t="s">
+      <c r="B217" s="11" t="s">
         <v>207</v>
       </c>
       <c r="C217" s="6" t="s">
@@ -4747,7 +4747,7 @@
       <c r="A218">
         <v>201</v>
       </c>
-      <c r="B218" s="5" t="s">
+      <c r="B218" s="11" t="s">
         <v>207</v>
       </c>
       <c r="C218" s="6" t="s">
@@ -4775,7 +4775,7 @@
       <c r="A220">
         <v>203</v>
       </c>
-      <c r="B220" s="5" t="s">
+      <c r="B220" s="11" t="s">
         <v>207</v>
       </c>
       <c r="C220" s="9" t="s">
@@ -4789,7 +4789,7 @@
       <c r="A221">
         <v>204</v>
       </c>
-      <c r="B221" s="5" t="s">
+      <c r="B221" s="11" t="s">
         <v>207</v>
       </c>
       <c r="C221" s="6" t="s">
@@ -4817,7 +4817,7 @@
       <c r="A223">
         <v>206</v>
       </c>
-      <c r="B223" s="5" t="s">
+      <c r="B223" s="11" t="s">
         <v>207</v>
       </c>
       <c r="C223" s="6" t="s">
@@ -4831,7 +4831,7 @@
       <c r="A224">
         <v>207</v>
       </c>
-      <c r="B224" s="5" t="s">
+      <c r="B224" s="11" t="s">
         <v>207</v>
       </c>
       <c r="C224" s="6" t="s">
@@ -4859,7 +4859,7 @@
       <c r="A226">
         <v>209</v>
       </c>
-      <c r="B226" s="5" t="s">
+      <c r="B226" s="11" t="s">
         <v>207</v>
       </c>
       <c r="C226" s="6" t="s">
@@ -4971,7 +4971,7 @@
       <c r="A234">
         <v>217</v>
       </c>
-      <c r="B234" s="5" t="s">
+      <c r="B234" s="11" t="s">
         <v>207</v>
       </c>
       <c r="C234" s="6" t="s">
@@ -4985,7 +4985,7 @@
       <c r="A235">
         <v>218</v>
       </c>
-      <c r="B235" s="5" t="s">
+      <c r="B235" s="11" t="s">
         <v>207</v>
       </c>
       <c r="C235" s="6" t="s">

</xml_diff>

<commit_message>
6th commit : 5th May 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3F91A3-87E6-46EE-AB80-076E8BC3BBC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D096059A-6E38-4A95-A987-70C2B5963B9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1521,7 +1521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1546,6 +1546,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1865,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" zoomScale="78" workbookViewId="0">
-      <selection activeCell="C234" sqref="C234"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="78" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3683,7 +3686,7 @@
       <c r="A139">
         <v>126</v>
       </c>
-      <c r="B139" s="8" t="s">
+      <c r="B139" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C139" s="6" t="s">
@@ -3697,7 +3700,7 @@
       <c r="A140">
         <v>127</v>
       </c>
-      <c r="B140" s="8" t="s">
+      <c r="B140" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C140" s="6" t="s">
@@ -3879,7 +3882,7 @@
       <c r="A153">
         <v>140</v>
       </c>
-      <c r="B153" s="8" t="s">
+      <c r="B153" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C153" s="6" t="s">
@@ -3893,7 +3896,7 @@
       <c r="A154">
         <v>141</v>
       </c>
-      <c r="B154" s="8" t="s">
+      <c r="B154" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C154" s="6" t="s">

</xml_diff>

<commit_message>
7th commit : 13th May 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D096059A-6E38-4A95-A987-70C2B5963B9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9087BAC-D113-425B-B654-F54C97DACB60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1868,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="78" workbookViewId="0">
-      <selection activeCell="C154" sqref="C154"/>
+    <sheetView tabSelected="1" topLeftCell="A287" zoomScale="78" workbookViewId="0">
+      <selection activeCell="C298" sqref="C298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3714,7 +3714,7 @@
       <c r="A141">
         <v>128</v>
       </c>
-      <c r="B141" s="8" t="s">
+      <c r="B141" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C141" s="6" t="s">
@@ -3728,7 +3728,7 @@
       <c r="A142">
         <v>129</v>
       </c>
-      <c r="B142" s="8" t="s">
+      <c r="B142" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C142" s="6" t="s">
@@ -3742,7 +3742,7 @@
       <c r="A143">
         <v>130</v>
       </c>
-      <c r="B143" s="8" t="s">
+      <c r="B143" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C143" s="6" t="s">
@@ -3756,7 +3756,7 @@
       <c r="A144">
         <v>131</v>
       </c>
-      <c r="B144" s="8" t="s">
+      <c r="B144" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C144" s="6" t="s">
@@ -3770,7 +3770,7 @@
       <c r="A145">
         <v>132</v>
       </c>
-      <c r="B145" s="8" t="s">
+      <c r="B145" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C145" s="6" t="s">
@@ -3812,7 +3812,7 @@
       <c r="A148">
         <v>135</v>
       </c>
-      <c r="B148" s="8" t="s">
+      <c r="B148" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C148" s="6" t="s">
@@ -3854,7 +3854,7 @@
       <c r="A151">
         <v>138</v>
       </c>
-      <c r="B151" s="8" t="s">
+      <c r="B151" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C151" s="6" t="s">
@@ -3924,7 +3924,7 @@
       <c r="A156">
         <v>143</v>
       </c>
-      <c r="B156" s="8" t="s">
+      <c r="B156" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C156" s="6" t="s">
@@ -4078,7 +4078,7 @@
       <c r="A167">
         <v>154</v>
       </c>
-      <c r="B167" s="8" t="s">
+      <c r="B167" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C167" s="6" t="s">
@@ -4092,7 +4092,7 @@
       <c r="A168">
         <v>155</v>
       </c>
-      <c r="B168" s="8" t="s">
+      <c r="B168" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C168" s="6" t="s">
@@ -5782,7 +5782,7 @@
       <c r="A296">
         <v>273</v>
       </c>
-      <c r="B296" s="5" t="s">
+      <c r="B296" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C296" s="6" t="s">
@@ -5810,7 +5810,7 @@
       <c r="A298">
         <v>275</v>
       </c>
-      <c r="B298" s="5" t="s">
+      <c r="B298" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C298" s="6" t="s">

</xml_diff>

<commit_message>
8th commit : 14th May 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9087BAC-D113-425B-B654-F54C97DACB60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82335C43-C7E1-4A2B-9C0E-36E4300478A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1868,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A287" zoomScale="78" workbookViewId="0">
-      <selection activeCell="C298" sqref="C298"/>
+    <sheetView tabSelected="1" topLeftCell="A297" zoomScale="78" workbookViewId="0">
+      <selection activeCell="C300" sqref="C300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5838,7 +5838,7 @@
       <c r="A300">
         <v>277</v>
       </c>
-      <c r="B300" s="5" t="s">
+      <c r="B300" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C300" s="6" t="s">
@@ -5852,7 +5852,7 @@
       <c r="A301">
         <v>278</v>
       </c>
-      <c r="B301" s="5" t="s">
+      <c r="B301" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C301" s="6" t="s">
@@ -5866,7 +5866,7 @@
       <c r="A302">
         <v>279</v>
       </c>
-      <c r="B302" s="5" t="s">
+      <c r="B302" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C302" s="6" t="s">
@@ -5908,7 +5908,7 @@
       <c r="A305">
         <v>282</v>
       </c>
-      <c r="B305" s="5" t="s">
+      <c r="B305" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C305" s="6" t="s">
@@ -5964,7 +5964,7 @@
       <c r="A309">
         <v>286</v>
       </c>
-      <c r="B309" s="5" t="s">
+      <c r="B309" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C309" s="9" t="s">
@@ -5978,7 +5978,7 @@
       <c r="A310">
         <v>287</v>
       </c>
-      <c r="B310" s="5" t="s">
+      <c r="B310" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C310" s="6" t="s">
@@ -6006,7 +6006,7 @@
       <c r="A312">
         <v>289</v>
       </c>
-      <c r="B312" s="5" t="s">
+      <c r="B312" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C312" s="6" t="s">
@@ -6034,7 +6034,7 @@
       <c r="A314">
         <v>291</v>
       </c>
-      <c r="B314" s="5" t="s">
+      <c r="B314" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C314" s="6" t="s">
@@ -6300,7 +6300,7 @@
       <c r="A333">
         <v>310</v>
       </c>
-      <c r="B333" s="5" t="s">
+      <c r="B333" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C333" s="6" t="s">

</xml_diff>

<commit_message>
9th commit : 20th May 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82335C43-C7E1-4A2B-9C0E-36E4300478A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F24D360-5759-458F-817A-13101F2C16D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1868,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A297" zoomScale="78" workbookViewId="0">
-      <selection activeCell="C300" sqref="C300"/>
+    <sheetView tabSelected="1" topLeftCell="A323" zoomScale="78" workbookViewId="0">
+      <selection activeCell="C340" sqref="C340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5796,7 +5796,7 @@
       <c r="A297">
         <v>274</v>
       </c>
-      <c r="B297" s="5" t="s">
+      <c r="B297" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C297" s="6" t="s">
@@ -6104,7 +6104,7 @@
       <c r="A319">
         <v>296</v>
       </c>
-      <c r="B319" s="5" t="s">
+      <c r="B319" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C319" s="6" t="s">
@@ -6146,7 +6146,7 @@
       <c r="A322">
         <v>299</v>
       </c>
-      <c r="B322" s="5" t="s">
+      <c r="B322" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C322" s="6" t="s">
@@ -6160,7 +6160,7 @@
       <c r="A323">
         <v>300</v>
       </c>
-      <c r="B323" s="5" t="s">
+      <c r="B323" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C323" s="6" t="s">
@@ -6174,7 +6174,7 @@
       <c r="A324">
         <v>301</v>
       </c>
-      <c r="B324" s="5" t="s">
+      <c r="B324" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C324" s="6" t="s">
@@ -6230,7 +6230,7 @@
       <c r="A328">
         <v>305</v>
       </c>
-      <c r="B328" s="5" t="s">
+      <c r="B328" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C328" s="6" t="s">
@@ -6258,7 +6258,7 @@
       <c r="A330">
         <v>307</v>
       </c>
-      <c r="B330" s="5" t="s">
+      <c r="B330" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C330" s="6" t="s">
@@ -6286,7 +6286,7 @@
       <c r="A332">
         <v>309</v>
       </c>
-      <c r="B332" s="5" t="s">
+      <c r="B332" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C332" s="6" t="s">
@@ -6322,7 +6322,7 @@
       <c r="A336">
         <v>311</v>
       </c>
-      <c r="B336" s="8" t="s">
+      <c r="B336" s="12" t="s">
         <v>324</v>
       </c>
       <c r="C336" s="6" t="s">
@@ -6336,7 +6336,7 @@
       <c r="A337">
         <v>312</v>
       </c>
-      <c r="B337" s="8" t="s">
+      <c r="B337" s="12" t="s">
         <v>324</v>
       </c>
       <c r="C337" s="6" t="s">
@@ -6378,7 +6378,7 @@
       <c r="A340">
         <v>315</v>
       </c>
-      <c r="B340" s="8" t="s">
+      <c r="B340" s="12" t="s">
         <v>324</v>
       </c>
       <c r="C340" s="6" t="s">

</xml_diff>

<commit_message>
10th commit : 21st May 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F24D360-5759-458F-817A-13101F2C16D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB075C27-43D2-47BC-AFCD-0ADF11CB250C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1868,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A323" zoomScale="78" workbookViewId="0">
-      <selection activeCell="C340" sqref="C340"/>
+    <sheetView tabSelected="1" topLeftCell="A334" zoomScale="78" workbookViewId="0">
+      <selection activeCell="C347" sqref="C347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6392,7 +6392,7 @@
       <c r="A341">
         <v>316</v>
       </c>
-      <c r="B341" s="8" t="s">
+      <c r="B341" s="12" t="s">
         <v>324</v>
       </c>
       <c r="C341" s="6" t="s">
@@ -6406,7 +6406,7 @@
       <c r="A342">
         <v>317</v>
       </c>
-      <c r="B342" s="8" t="s">
+      <c r="B342" s="12" t="s">
         <v>324</v>
       </c>
       <c r="C342" s="6" t="s">
@@ -6420,7 +6420,7 @@
       <c r="A343">
         <v>318</v>
       </c>
-      <c r="B343" s="8" t="s">
+      <c r="B343" s="12" t="s">
         <v>324</v>
       </c>
       <c r="C343" s="6" t="s">
@@ -6448,7 +6448,7 @@
       <c r="A345">
         <v>320</v>
       </c>
-      <c r="B345" s="8" t="s">
+      <c r="B345" s="12" t="s">
         <v>324</v>
       </c>
       <c r="C345" s="6" t="s">
@@ -6462,7 +6462,7 @@
       <c r="A346">
         <v>321</v>
       </c>
-      <c r="B346" s="8" t="s">
+      <c r="B346" s="12" t="s">
         <v>324</v>
       </c>
       <c r="C346" s="6" t="s">
@@ -6476,7 +6476,7 @@
       <c r="A347">
         <v>322</v>
       </c>
-      <c r="B347" s="8" t="s">
+      <c r="B347" s="12" t="s">
         <v>324</v>
       </c>
       <c r="C347" s="6" t="s">
@@ -6490,7 +6490,7 @@
       <c r="A348">
         <v>323</v>
       </c>
-      <c r="B348" s="8" t="s">
+      <c r="B348" s="12" t="s">
         <v>324</v>
       </c>
       <c r="C348" s="6" t="s">
@@ -6504,7 +6504,7 @@
       <c r="A349">
         <v>324</v>
       </c>
-      <c r="B349" s="8" t="s">
+      <c r="B349" s="12" t="s">
         <v>324</v>
       </c>
       <c r="C349" s="6" t="s">

</xml_diff>

<commit_message>
11th commit : 23rd May 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB075C27-43D2-47BC-AFCD-0ADF11CB250C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0368F671-FF64-4B19-8ACD-398F92426563}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1868,7 +1868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A334" zoomScale="78" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A364" zoomScale="78" workbookViewId="0">
       <selection activeCell="C347" sqref="C347"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
12th commit : 27th May 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0368F671-FF64-4B19-8ACD-398F92426563}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897AF186-146E-4F8C-9FF7-C105CFC0CB65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1868,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A364" zoomScale="78" workbookViewId="0">
-      <selection activeCell="C347" sqref="C347"/>
+    <sheetView tabSelected="1" topLeftCell="A350" zoomScale="78" workbookViewId="0">
+      <selection activeCell="C357" sqref="C357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5508,7 +5508,7 @@
       <c r="A275">
         <v>254</v>
       </c>
-      <c r="B275" s="5" t="s">
+      <c r="B275" s="11" t="s">
         <v>265</v>
       </c>
       <c r="C275" s="6" t="s">
@@ -5522,7 +5522,7 @@
       <c r="A276">
         <v>255</v>
       </c>
-      <c r="B276" s="5" t="s">
+      <c r="B276" s="11" t="s">
         <v>265</v>
       </c>
       <c r="C276" s="6" t="s">
@@ -5564,7 +5564,7 @@
       <c r="A279">
         <v>258</v>
       </c>
-      <c r="B279" s="5" t="s">
+      <c r="B279" s="11" t="s">
         <v>265</v>
       </c>
       <c r="C279" s="6" t="s">
@@ -6582,7 +6582,7 @@
       <c r="A356">
         <v>329</v>
       </c>
-      <c r="B356" s="8" t="s">
+      <c r="B356" s="12" t="s">
         <v>343</v>
       </c>
       <c r="C356" s="6" t="s">
@@ -6596,7 +6596,7 @@
       <c r="A357">
         <v>330</v>
       </c>
-      <c r="B357" s="8" t="s">
+      <c r="B357" s="12" t="s">
         <v>343</v>
       </c>
       <c r="C357" s="6" t="s">
@@ -7262,7 +7262,7 @@
       <c r="A406">
         <v>377</v>
       </c>
-      <c r="B406" s="8" t="s">
+      <c r="B406" s="12" t="s">
         <v>387</v>
       </c>
       <c r="C406" s="6" t="s">

</xml_diff>

<commit_message>
13th commit : 28th May 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897AF186-146E-4F8C-9FF7-C105CFC0CB65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113DD22D-FEA9-4C65-8B5C-6913BFDB73BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1868,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A350" zoomScale="78" workbookViewId="0">
-      <selection activeCell="C357" sqref="C357"/>
+    <sheetView tabSelected="1" topLeftCell="A355" zoomScale="78" workbookViewId="0">
+      <selection activeCell="C367" sqref="C367"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6610,7 +6610,7 @@
       <c r="A358">
         <v>331</v>
       </c>
-      <c r="B358" s="8" t="s">
+      <c r="B358" s="12" t="s">
         <v>343</v>
       </c>
       <c r="C358" s="6" t="s">
@@ -6624,7 +6624,7 @@
       <c r="A359">
         <v>332</v>
       </c>
-      <c r="B359" s="8" t="s">
+      <c r="B359" s="12" t="s">
         <v>343</v>
       </c>
       <c r="C359" s="6" t="s">
@@ -6638,7 +6638,7 @@
       <c r="A360">
         <v>333</v>
       </c>
-      <c r="B360" s="8" t="s">
+      <c r="B360" s="12" t="s">
         <v>343</v>
       </c>
       <c r="C360" s="6" t="s">
@@ -6736,7 +6736,7 @@
       <c r="A367">
         <v>340</v>
       </c>
-      <c r="B367" s="8" t="s">
+      <c r="B367" s="12" t="s">
         <v>343</v>
       </c>
       <c r="C367" s="6" t="s">
@@ -6750,7 +6750,7 @@
       <c r="A368">
         <v>341</v>
       </c>
-      <c r="B368" s="8" t="s">
+      <c r="B368" s="12" t="s">
         <v>343</v>
       </c>
       <c r="C368" s="6" t="s">

</xml_diff>

<commit_message>
14th commit : 1st June 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113DD22D-FEA9-4C65-8B5C-6913BFDB73BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C074EFE1-8C09-4784-8F72-1D4BCD08643E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1868,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A355" zoomScale="78" workbookViewId="0">
-      <selection activeCell="C367" sqref="C367"/>
+    <sheetView tabSelected="1" topLeftCell="A374" zoomScale="78" workbookViewId="0">
+      <selection activeCell="C381" sqref="C381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6834,7 +6834,7 @@
       <c r="A374">
         <v>347</v>
       </c>
-      <c r="B374" s="8" t="s">
+      <c r="B374" s="12" t="s">
         <v>343</v>
       </c>
       <c r="C374" s="6" t="s">
@@ -6932,7 +6932,7 @@
       <c r="A381">
         <v>354</v>
       </c>
-      <c r="B381" s="8" t="s">
+      <c r="B381" s="12" t="s">
         <v>343</v>
       </c>
       <c r="C381" s="6" t="s">

</xml_diff>

<commit_message>
15th commit : 1st June 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C074EFE1-8C09-4784-8F72-1D4BCD08643E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112A0483-D5F5-4BE0-93EA-7DFFDEA30006}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1868,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A374" zoomScale="78" workbookViewId="0">
-      <selection activeCell="C381" sqref="C381"/>
+    <sheetView tabSelected="1" topLeftCell="A368" zoomScale="78" workbookViewId="0">
+      <selection activeCell="C376" sqref="C376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6862,7 +6862,7 @@
       <c r="A376">
         <v>349</v>
       </c>
-      <c r="B376" s="8" t="s">
+      <c r="B376" s="12" t="s">
         <v>343</v>
       </c>
       <c r="C376" s="6" t="s">
@@ -6946,7 +6946,7 @@
       <c r="A382">
         <v>355</v>
       </c>
-      <c r="B382" s="8" t="s">
+      <c r="B382" s="12" t="s">
         <v>343</v>
       </c>
       <c r="C382" s="6" t="s">

</xml_diff>

<commit_message>
16th commit : 10th November 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\C++_450\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\DSA\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112A0483-D5F5-4BE0-93EA-7DFFDEA30006}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78945093-9E41-4367-BBEB-1C52D5800FE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1868,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A368" zoomScale="78" workbookViewId="0">
-      <selection activeCell="C376" sqref="C376"/>
+    <sheetView tabSelected="1" topLeftCell="A389" zoomScale="78" workbookViewId="0">
+      <selection activeCell="B410" sqref="B410"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -7298,7 +7298,7 @@
       <c r="A410">
         <v>379</v>
       </c>
-      <c r="B410" s="5" t="s">
+      <c r="B410" s="11" t="s">
         <v>393</v>
       </c>
       <c r="C410" s="6" t="s">

</xml_diff>

<commit_message>
17th commit : 13th November 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\DSA\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78945093-9E41-4367-BBEB-1C52D5800FE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0644E64-B879-489B-8FAF-521733788AEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1868,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A389" zoomScale="78" workbookViewId="0">
-      <selection activeCell="B410" sqref="B410"/>
+    <sheetView tabSelected="1" topLeftCell="A447" zoomScale="78" workbookViewId="0">
+      <selection activeCell="C434" sqref="C434"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -7312,7 +7312,7 @@
       <c r="A411">
         <v>380</v>
       </c>
-      <c r="B411" s="5" t="s">
+      <c r="B411" s="11" t="s">
         <v>393</v>
       </c>
       <c r="C411" s="6" t="s">
@@ -7452,7 +7452,7 @@
       <c r="A421">
         <v>390</v>
       </c>
-      <c r="B421" s="5" t="s">
+      <c r="B421" s="11" t="s">
         <v>393</v>
       </c>
       <c r="C421" s="6" t="s">
@@ -7634,7 +7634,7 @@
       <c r="A434">
         <v>403</v>
       </c>
-      <c r="B434" s="5" t="s">
+      <c r="B434" s="11" t="s">
         <v>393</v>
       </c>
       <c r="C434" s="6" t="s">
@@ -7942,7 +7942,7 @@
       <c r="A456">
         <v>425</v>
       </c>
-      <c r="B456" s="5" t="s">
+      <c r="B456" s="11" t="s">
         <v>393</v>
       </c>
       <c r="C456" s="6" t="s">

</xml_diff>

<commit_message>
18th commit : 14th November 2022
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\DSA\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0644E64-B879-489B-8FAF-521733788AEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E0139D-1D29-4052-A249-9C05977843BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1868,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A447" zoomScale="78" workbookViewId="0">
-      <selection activeCell="C434" sqref="C434"/>
+    <sheetView tabSelected="1" topLeftCell="A435" zoomScale="78" workbookViewId="0">
+      <selection activeCell="C420" sqref="C420"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -7508,7 +7508,7 @@
       <c r="A425">
         <v>394</v>
       </c>
-      <c r="B425" s="5" t="s">
+      <c r="B425" s="11" t="s">
         <v>393</v>
       </c>
       <c r="C425" s="6" t="s">

</xml_diff>

<commit_message>
24th commit : 13th March 2023
</commit_message>
<xml_diff>
--- a/.FINAL450.xlsx
+++ b/.FINAL450.xlsx
@@ -8,22 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NitSh\Desktop\Programings\DSA\C++_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E0139D-1D29-4052-A249-9C05977843BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA347C45-FD14-43F9-95AE-8BE72429EA2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="7980" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1868,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A435" zoomScale="78" workbookViewId="0">
-      <selection activeCell="C420" sqref="C420"/>
+    <sheetView tabSelected="1" topLeftCell="B48" zoomScale="78" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2571,7 +2566,7 @@
       <c r="A56">
         <v>47</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C56" s="6" t="s">
@@ -2585,7 +2580,7 @@
       <c r="A57">
         <v>48</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C57" s="6" t="s">
@@ -3178,7 +3173,7 @@
       <c r="A101">
         <v>90</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="11" t="s">
         <v>97</v>
       </c>
       <c r="C101" s="6" t="s">
@@ -3192,7 +3187,7 @@
       <c r="A102">
         <v>91</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="11" t="s">
         <v>97</v>
       </c>
       <c r="C102" s="6" t="s">
@@ -3206,7 +3201,7 @@
       <c r="A103">
         <v>92</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="11" t="s">
         <v>97</v>
       </c>
       <c r="C103" s="6" t="s">
@@ -3220,7 +3215,7 @@
       <c r="A104">
         <v>93</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B104" s="11" t="s">
         <v>97</v>
       </c>
       <c r="C104" s="6" t="s">
@@ -3500,7 +3495,7 @@
       <c r="A124">
         <v>113</v>
       </c>
-      <c r="B124" s="5" t="s">
+      <c r="B124" s="11" t="s">
         <v>97</v>
       </c>
       <c r="C124" s="6" t="s">
@@ -3514,7 +3509,7 @@
       <c r="A125">
         <v>114</v>
       </c>
-      <c r="B125" s="5" t="s">
+      <c r="B125" s="11" t="s">
         <v>97</v>
       </c>
       <c r="C125" s="6" t="s">
@@ -3528,7 +3523,7 @@
       <c r="A126">
         <v>115</v>
       </c>
-      <c r="B126" s="5" t="s">
+      <c r="B126" s="11" t="s">
         <v>97</v>
       </c>
       <c r="C126" s="6" t="s">
@@ -3584,7 +3579,7 @@
       <c r="A130">
         <v>119</v>
       </c>
-      <c r="B130" s="5" t="s">
+      <c r="B130" s="11" t="s">
         <v>97</v>
       </c>
       <c r="C130" s="6" t="s">

</xml_diff>